<commit_message>
Small changes to clean for next session
</commit_message>
<xml_diff>
--- a/Architecture_tables.xlsx
+++ b/Architecture_tables.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12315" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12315" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FLMALS" sheetId="1" r:id="rId1"/>
     <sheet name="DAYLP" sheetId="7" r:id="rId2"/>
     <sheet name="MALDIS" sheetId="6" r:id="rId3"/>
     <sheet name="FLMALN" sheetId="2" r:id="rId4"/>
-    <sheet name="GroMALP" sheetId="5" r:id="rId5"/>
-    <sheet name="GroMALC" sheetId="4" r:id="rId6"/>
+    <sheet name="FLMALC" sheetId="4" r:id="rId5"/>
+    <sheet name="MALGro" sheetId="5" r:id="rId6"/>
     <sheet name="equations exploration" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="251">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -171,15 +171,9 @@
     <t>OUT</t>
   </si>
   <si>
-    <t>Ks</t>
-  </si>
-  <si>
     <t>half saturation N uptake</t>
   </si>
   <si>
-    <t>Jmax</t>
-  </si>
-  <si>
     <t>maximum N uptake rate</t>
   </si>
   <si>
@@ -234,16 +228,10 @@
     <t>P:C ratio in structural mass</t>
   </si>
   <si>
-    <t>kp</t>
-  </si>
-  <si>
     <t>half saturation P uptake</t>
   </si>
   <si>
     <t>maximum P uptake rate</t>
-  </si>
-  <si>
-    <t>gP/DM day</t>
   </si>
   <si>
     <t>Is</t>
@@ -1191,11 +1179,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="421215808"/>
-        <c:axId val="421218944"/>
+        <c:axId val="629028192"/>
+        <c:axId val="629021136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="421215808"/>
+        <c:axId val="629028192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,12 +1193,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421218944"/>
+        <c:crossAx val="629021136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="421218944"/>
+        <c:axId val="629021136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,7 +1209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421215808"/>
+        <c:crossAx val="629028192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1580,14 +1568,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1595,7 +1583,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1618,10 +1606,10 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1636,7 +1624,7 @@
         <v>-999</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>30</v>
@@ -1655,7 +1643,7 @@
         <v>-999</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>11</v>
@@ -1674,7 +1662,7 @@
         <v>-999</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>12</v>
@@ -1693,7 +1681,7 @@
         <v>-999</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>13</v>
@@ -1706,16 +1694,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B9" s="8">
         <v>-999</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>31</v>
@@ -1731,7 +1719,7 @@
         <v>0.01</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>5</v>
@@ -1750,7 +1738,7 @@
         <v>0.01</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>6</v>
@@ -1763,76 +1751,76 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="5">
         <v>-999</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B13" s="5">
         <v>-999</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B14" s="5">
         <v>-999</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B15" s="5">
         <v>-999</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1845,7 +1833,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>16</v>
@@ -1864,7 +1852,7 @@
         <v>0.1085</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>19</v>
@@ -1883,7 +1871,7 @@
         <v>0.03</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -1903,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>23</v>
@@ -1922,7 +1910,7 @@
         <v>0.85</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>26</v>
@@ -1941,7 +1929,7 @@
         <v>0.3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>27</v>
@@ -1961,10 +1949,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>38</v>
@@ -1974,16 +1962,16 @@
     </row>
     <row r="23" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B23" s="8">
         <v>0.5</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>36</v>
@@ -1993,16 +1981,16 @@
     </row>
     <row r="24" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B24" s="8">
         <v>0.2</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>36</v>
@@ -2012,16 +2000,16 @@
     </row>
     <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B25" s="8">
         <v>0.02</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>36</v>
@@ -2031,16 +2019,16 @@
     </row>
     <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B26" s="8">
         <v>0.75</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>36</v>
@@ -2050,16 +2038,16 @@
     </row>
     <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B27" s="8">
         <v>0.25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>36</v>
@@ -2069,16 +2057,16 @@
     </row>
     <row r="28" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B28" s="8">
         <v>-999</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>38</v>
@@ -2088,38 +2076,38 @@
     </row>
     <row r="29" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B29" s="8">
         <v>-999</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B30" s="8">
         <v>-999</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -2127,10 +2115,10 @@
     <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -2140,10 +2128,10 @@
     <row r="32" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -2152,14 +2140,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>31</v>
@@ -2169,14 +2157,14 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>32</v>
@@ -2186,14 +2174,14 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>33</v>
@@ -2203,14 +2191,14 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>34</v>
@@ -2220,14 +2208,14 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>36</v>
@@ -2237,14 +2225,14 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>36</v>
@@ -2254,14 +2242,14 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>36</v>
@@ -2271,14 +2259,14 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>36</v>
@@ -2288,14 +2276,14 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>36</v>
@@ -2305,75 +2293,75 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
@@ -2383,10 +2371,10 @@
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
@@ -2395,119 +2383,119 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
@@ -2523,211 +2511,213 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="5">
+        <v>52</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B5">
-        <v>-999</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B8" s="5">
+        <v>86400</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E8" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B6">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" t="s">
-        <v>215</v>
-      </c>
-      <c r="E6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E11" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B8">
-        <v>86400</v>
-      </c>
-      <c r="C8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" t="s">
-        <v>211</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" t="s">
-        <v>213</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>204</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2750,14 +2740,14 @@
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2765,7 +2755,7 @@
     </row>
     <row r="2" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2788,10 +2778,10 @@
     <row r="4" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2800,16 +2790,16 @@
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" s="8">
         <v>-999</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>38</v>
@@ -2819,57 +2809,57 @@
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B6" s="8">
         <v>-999</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B7" s="8">
         <v>-999</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B8" s="8">
         <v>-999</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -2882,7 +2872,7 @@
         <v>-999</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>30</v>
@@ -2899,7 +2889,7 @@
         <v>-999</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -2916,7 +2906,7 @@
         <v>-999</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
@@ -2933,7 +2923,7 @@
         <v>-999</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>13</v>
@@ -2944,45 +2934,45 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B13" s="5">
         <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B14" s="5">
         <v>100</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -2992,10 +2982,10 @@
     <row r="16" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -3004,13 +2994,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>31</v>
@@ -3018,28 +3008,28 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>36</v>
@@ -3057,35 +3047,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3104,10 +3094,10 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -3120,7 +3110,7 @@
         <v>-999</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3142,7 +3132,7 @@
         <v>-999</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -3164,10 +3154,10 @@
         <v>-999</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>43</v>
@@ -3183,10 +3173,10 @@
         <v>-999</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>43</v>
@@ -3196,35 +3186,35 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="5">
         <v>-999</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B10" s="8">
         <v>-999</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>31</v>
@@ -3243,7 +3233,7 @@
         <v>0.01</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>5</v>
@@ -3265,7 +3255,7 @@
         <v>0.1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>45</v>
@@ -3285,7 +3275,7 @@
         <v>1E-3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>6</v>
@@ -3301,16 +3291,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="5">
         <v>0.01</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>33</v>
@@ -3321,19 +3311,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B15" s="5">
         <v>0.5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F15" s="5">
         <v>0.2</v>
@@ -3343,13 +3333,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B16" s="5">
         <v>0.2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>44</v>
@@ -3365,16 +3355,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B17" s="5">
         <v>0.02</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>33</v>
@@ -3387,16 +3377,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B18" s="5">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>43</v>
@@ -3410,19 +3400,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B19" s="5">
         <v>5.5999999999999999E-3</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F19" s="5">
         <f>0.00014*24/0.6</f>
@@ -3433,19 +3423,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B20" s="5">
         <v>5.5999999999999999E-3</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F20" s="5">
         <v>-999</v>
@@ -3455,19 +3445,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B21" s="5">
         <v>5.5999999999999995E-4</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F21" s="5">
         <v>-999</v>
@@ -3477,19 +3467,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5">
         <v>-999</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="6">
         <v>0.03</v>
@@ -3499,33 +3489,33 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="6">
         <v>0.03</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B24" s="8">
         <v>-999</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>38</v>
@@ -3533,46 +3523,46 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B25" s="8">
         <v>-999</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B26" s="8">
         <v>-999</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -3580,10 +3570,10 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>36</v>
@@ -3591,14 +3581,14 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>36</v>
@@ -3606,41 +3596,41 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D31" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -3648,57 +3638,57 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3753,10 +3743,374 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6">
+        <v>-999</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="5">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="5">
+        <f>285</f>
+        <v>285</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="5">
+        <f>290</f>
+        <v>290</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11">
+        <f>1694.4-273</f>
+        <v>1421.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="5">
+        <f>25924</f>
+        <v>25924</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="5">
+        <v>27774</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="5">
+        <v>11033</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="5">
+        <f>0.0000375*(1/F3)*24</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="6">
+        <v>200</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3815,17 +4169,11 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="5">
-        <v>-999</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
         <f>6*0.6</f>
@@ -3834,23 +4182,17 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="5">
-        <v>-999</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -3859,125 +4201,65 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.01</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.01</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.2</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="5">
-        <f>4*F10*0.001</f>
-        <v>5.6000000000000001E-2</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="5">
-        <f>0.00014*24/0.6</f>
-        <v>5.5999999999999999E-3</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="5">
-        <v>-999</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.03</v>
-      </c>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -3985,9 +4267,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -4001,370 +4281,6 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="5">
-        <v>-999</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="6">
-        <v>-999</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="5">
-        <v>-999</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="5">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="5">
-        <f>285</f>
-        <v>285</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="5">
-        <f>290</f>
-        <v>290</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11">
-        <f>1694.4-273</f>
-        <v>1421.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="5">
-        <f>25924</f>
-        <v>25924</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="5">
-        <v>27774</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="5">
-        <v>11033</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="5">
-        <v>-999</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="5">
-        <v>-999</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="5">
-        <f>0.0000375*(1/F3)*24</f>
-        <v>1.5E-3</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="6">
-        <v>200</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4383,16 +4299,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B1">
         <v>0.1085</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4412,7 +4328,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B3">
         <v>6</v>

</xml_diff>